<commit_message>
13 minutes for 2-17-2021.
</commit_message>
<xml_diff>
--- a/Time Tracking.xlsx
+++ b/Time Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\r\coding-sessions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3959CFA3-716B-40E7-926A-8D642E0C4DEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1EE12E-C13B-4083-9B10-66715A038CD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24810" yWindow="4155" windowWidth="21600" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,15 +407,15 @@
   <dimension ref="A2:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -450,7 +450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -464,21 +464,23 @@
       <c r="D3" s="3">
         <v>24</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3">
+        <v>13</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="4">
         <f t="shared" ref="J3:J48" si="0">SUM(C3:I3)</f>
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="K3" s="5">
         <f>J3/60</f>
-        <v>0.93333333333333335</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -501,7 +503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -524,7 +526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -547,7 +549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -570,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -593,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -616,7 +618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -639,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -662,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -685,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -708,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -731,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -754,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -770,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -786,7 +788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -802,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -818,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -834,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -850,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -866,7 +868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -882,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -898,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -914,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -930,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -946,7 +948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -962,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -978,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -994,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1010,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1026,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1042,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1058,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1074,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1090,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1106,7 +1108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1122,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1138,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1154,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1170,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1186,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1202,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1218,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1234,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1250,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1266,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1282,14 +1284,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="10:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J49" s="5">
         <f>SUM(J3:J48)</f>
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="K49" s="5">
         <f>SUM(K3:K48)</f>
-        <v>0.93333333333333335</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Friday (2/26) time tracking.
</commit_message>
<xml_diff>
--- a/Time Tracking.xlsx
+++ b/Time Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\r\coding-sessions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEE7754-9295-426F-B5FA-25F5D26B1017}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84956161-0D55-4D2D-A050-2F6EF0AD37D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60075" yWindow="3165" windowWidth="21360" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24525" yWindow="1560" windowWidth="18675" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,15 +407,15 @@
   <dimension ref="A2:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.3984375" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -450,7 +450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -482,7 +482,7 @@
         <v>1.8333333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -490,22 +490,26 @@
         <v>44249</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>15</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3">
+        <v>55</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" ref="K4:K48" si="1">J4/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -528,7 +532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -551,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -574,7 +578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -597,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -620,7 +624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -643,7 +647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -666,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -689,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -712,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -735,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -758,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -774,7 +778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -790,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -806,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -822,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -838,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -854,7 +858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -870,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -886,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -902,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -918,7 +922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -934,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -950,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -966,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -982,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -998,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1014,7 +1018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1030,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1046,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1062,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1078,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1094,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1110,7 +1114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1126,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1142,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1158,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1190,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1206,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1222,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1254,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1270,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1286,14 +1290,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="10:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J49" s="5">
         <f>SUM(J3:J48)</f>
-        <v>110</v>
+        <v>180</v>
       </c>
       <c r="K49" s="5">
         <f>SUM(K3:K48)</f>
-        <v>1.8333333333333333</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spend 41 min on chapter 14: Change.
</commit_message>
<xml_diff>
--- a/Time Tracking.xlsx
+++ b/Time Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\r\coding-sessions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84956161-0D55-4D2D-A050-2F6EF0AD37D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A37EB0A-3152-4127-98BD-627055EA92F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24525" yWindow="1560" windowWidth="18675" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A2:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,17 +519,19 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3">
+        <v>41</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.68333333333333335</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1293,11 +1295,11 @@
     <row r="49" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J49" s="5">
         <f>SUM(J3:J48)</f>
-        <v>180</v>
+        <v>221</v>
       </c>
       <c r="K49" s="5">
         <f>SUM(K3:K48)</f>
-        <v>3</v>
+        <v>3.6833333333333336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Loagged time 20 min.
</commit_message>
<xml_diff>
--- a/Time Tracking.xlsx
+++ b/Time Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\r\coding-sessions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A37EB0A-3152-4127-98BD-627055EA92F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88A51BC-1FA3-4BA3-B979-64D40ABABC03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A2:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,7 +541,9 @@
       <c r="B6" s="2">
         <v>44263</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3">
+        <v>20</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -550,11 +552,11 @@
       <c r="I6" s="3"/>
       <c r="J6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1295,11 +1297,11 @@
     <row r="49" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J49" s="5">
         <f>SUM(J3:J48)</f>
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="K49" s="5">
         <f>SUM(K3:K48)</f>
-        <v>3.6833333333333336</v>
+        <v>4.0166666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Time spent: 20 min.
</commit_message>
<xml_diff>
--- a/Time Tracking.xlsx
+++ b/Time Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\r\coding-sessions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88A51BC-1FA3-4BA3-B979-64D40ABABC03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F283F7-3202-448D-83AC-BF0274D0121D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A2:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,7 +544,9 @@
       <c r="C6" s="3">
         <v>20</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>20</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -552,11 +554,11 @@
       <c r="I6" s="3"/>
       <c r="J6" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1297,11 +1299,11 @@
     <row r="49" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J49" s="5">
         <f>SUM(J3:J48)</f>
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="K49" s="5">
         <f>SUM(K3:K48)</f>
-        <v>4.0166666666666666</v>
+        <v>4.3500000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Notes test files. Recorded time: 21 min.
</commit_message>
<xml_diff>
--- a/Time Tracking.xlsx
+++ b/Time Tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\r\coding-sessions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F283F7-3202-448D-83AC-BF0274D0121D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BA6654-FF4D-4DEC-898D-B5A34BAA8EFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25380" yWindow="3585" windowWidth="21600" windowHeight="12855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A2:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,18 +547,20 @@
       <c r="D6" s="3">
         <v>20</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3">
+        <v>21</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="4">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>1.0166666666666666</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1299,11 +1301,11 @@
     <row r="49" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J49" s="5">
         <f>SUM(J3:J48)</f>
-        <v>261</v>
+        <v>282</v>
       </c>
       <c r="K49" s="5">
         <f>SUM(K3:K48)</f>
-        <v>4.3500000000000005</v>
+        <v>4.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tracked time 11 min.
</commit_message>
<xml_diff>
--- a/Time Tracking.xlsx
+++ b/Time Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\r\coding-sessions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD21ACE3-9F05-4665-9EE5-B504465AA4BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DD7EBB-B6C0-4736-AE43-1ED59B6D03BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="A2:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -615,17 +615,19 @@
         <v>24</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3">
+        <v>11</v>
+      </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="4">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="1"/>
-        <v>0.95</v>
+        <v>1.1333333333333333</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -1320,11 +1322,11 @@
     <row r="49" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J49" s="5">
         <f>SUM(J3:J48)</f>
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="K49" s="6">
         <f>SUM(K3:K48)</f>
-        <v>7.6166666666666671</v>
+        <v>7.8000000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tracked time: 25 min.
</commit_message>
<xml_diff>
--- a/Time Tracking.xlsx
+++ b/Time Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\r\coding-sessions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DD7EBB-B6C0-4736-AE43-1ED59B6D03BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F135295-071F-4870-A298-CF5C11322F04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,15 +414,15 @@
   <dimension ref="A2:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -457,7 +457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -489,7 +489,7 @@
         <v>1.8333333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -516,7 +516,7 @@
         <v>1.1666666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -541,7 +541,7 @@
         <v>0.68333333333333335</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -574,7 +574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -601,7 +601,7 @@
         <v>0.98333333333333328</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -630,14 +630,16 @@
         <v>1.1333333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>44284</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3">
+        <v>25</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -646,14 +648,14 @@
       <c r="I9" s="3"/>
       <c r="J9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -676,7 +678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -699,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -722,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -745,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -768,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -791,7 +793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -807,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -823,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -839,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -855,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -871,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -887,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -903,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -919,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -935,7 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -951,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -967,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -983,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -999,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1015,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1031,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1047,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1063,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1079,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1095,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1111,7 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1127,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1143,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1159,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1175,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1191,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1207,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1223,7 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1239,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1255,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1271,7 +1273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1287,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1303,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1319,14 +1321,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="10:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J49" s="5">
         <f>SUM(J3:J48)</f>
-        <v>468</v>
+        <v>493</v>
       </c>
       <c r="K49" s="6">
         <f>SUM(K3:K48)</f>
-        <v>7.8000000000000007</v>
+        <v>8.2166666666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>